<commit_message>
S&P 500 Excel File
</commit_message>
<xml_diff>
--- a/Excel/SP500_excel.xlsx
+++ b/Excel/SP500_excel.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>-0.1%</t>
+          <t>-0.51%</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -584,7 +584,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.87%</t>
+          <t>0.81%</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2.49%</t>
+          <t>3.01%</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -688,7 +688,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2.39%</t>
+          <t>2.27%</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -740,7 +740,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2.33%</t>
+          <t>2.67%</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -792,7 +792,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1.37%</t>
+          <t>1.21%</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2.12%</t>
+          <t>2.08%</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>-0.67%</t>
+          <t>-0.4%</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -948,7 +948,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.62%</t>
+          <t>0.56%</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.57%</t>
+          <t>0.52%</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2.34%</t>
+          <t>2.41%</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>-0.13%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>-0.48%</t>
+          <t>-0.57%</t>
         </is>
       </c>
       <c r="J14" t="n">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.19%</t>
+          <t>0.61%</t>
         </is>
       </c>
       <c r="J15" t="n">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1.06%</t>
+          <t>0.65%</t>
         </is>
       </c>
       <c r="J16" t="n">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>-0.47%</t>
+          <t>-0.98%</t>
         </is>
       </c>
       <c r="J17" t="n">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1.17%</t>
+          <t>1.19%</t>
         </is>
       </c>
       <c r="J18" t="n">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.15%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J19" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>-0.82%</t>
+          <t>-0.85%</t>
         </is>
       </c>
       <c r="J20" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2.52%</t>
+          <t>2.56%</t>
         </is>
       </c>
       <c r="J22" t="n">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1.54%</t>
+          <t>1.94%</t>
         </is>
       </c>
       <c r="J23" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>-0.76%</t>
+          <t>-0.67%</t>
         </is>
       </c>
       <c r="J24" t="n">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1.29%</t>
+          <t>1.35%</t>
         </is>
       </c>
       <c r="J25" t="n">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.27%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J26" t="n">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>-0.11%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J27" t="n">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>-0.83%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J28" t="n">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.37%</t>
+          <t>1.72%</t>
         </is>
       </c>
       <c r="J29" t="n">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1.45%</t>
+          <t>1.54%</t>
         </is>
       </c>
       <c r="J30" t="n">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.51%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J31" t="n">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>-0.18%</t>
+          <t>-0.72%</t>
         </is>
       </c>
       <c r="J32" t="n">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>-0.24%</t>
+          <t>-0.29%</t>
         </is>
       </c>
       <c r="J33" t="n">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2.06%</t>
+          <t>2.1%</t>
         </is>
       </c>
       <c r="J34" t="n">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.55%</t>
+          <t>0.69%</t>
         </is>
       </c>
       <c r="J35" t="n">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.64%</t>
+          <t>2.04%</t>
         </is>
       </c>
       <c r="J36" t="n">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>-0.48%</t>
+          <t>-0.58%</t>
         </is>
       </c>
       <c r="J37" t="n">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>-0.68%</t>
+          <t>-0.49%</t>
         </is>
       </c>
       <c r="J38" t="n">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>-1.0%</t>
+          <t>-2.17%</t>
         </is>
       </c>
       <c r="J39" t="n">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>0.39%</t>
+          <t>0.93%</t>
         </is>
       </c>
       <c r="J40" t="n">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>-0.22%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J41" t="n">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>-0.11%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J42" t="n">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>-1.49%</t>
+          <t>-2.0%</t>
         </is>
       </c>
       <c r="J43" t="n">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>0.31%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J44" t="n">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>1.32%</t>
+          <t>1.31%</t>
         </is>
       </c>
       <c r="J45" t="n">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>0.17%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J46" t="n">
@@ -2872,7 +2872,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>-0.72%</t>
+          <t>-0.88%</t>
         </is>
       </c>
       <c r="J47" t="n">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>-0.13%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J48" t="n">
@@ -2976,7 +2976,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>-0.6%</t>
+          <t>-0.7%</t>
         </is>
       </c>
       <c r="J49" t="n">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>-0.08%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J50" t="n">
@@ -3080,7 +3080,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>0.52%</t>
+          <t>3.85%</t>
         </is>
       </c>
       <c r="J51" t="n">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>-2.73%</t>
+          <t>-3.1%</t>
         </is>
       </c>
       <c r="J52" t="n">
@@ -3184,7 +3184,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>-0.61%</t>
+          <t>-0.6%</t>
         </is>
       </c>
       <c r="J53" t="n">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>-0.98%</t>
+          <t>-1.1%</t>
         </is>
       </c>
       <c r="J54" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>0.31%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J55" t="n">
@@ -3340,7 +3340,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>-0.55%</t>
+          <t>-0.72%</t>
         </is>
       </c>
       <c r="J56" t="n">
@@ -3392,7 +3392,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>-0.04%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J57" t="n">
@@ -3444,7 +3444,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>-0.8%</t>
+          <t>-0.82%</t>
         </is>
       </c>
       <c r="J58" t="n">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>-0.36%</t>
+          <t>-0.35%</t>
         </is>
       </c>
       <c r="J59" t="n">
@@ -3548,7 +3548,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>0.14%</t>
         </is>
       </c>
       <c r="J60" t="n">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>0.1%</t>
+          <t>0.23%</t>
         </is>
       </c>
       <c r="J61" t="n">
@@ -3652,7 +3652,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>-1.11%</t>
+          <t>-1.23%</t>
         </is>
       </c>
       <c r="J62" t="n">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>-0.8%</t>
+          <t>-0.87%</t>
         </is>
       </c>
       <c r="J63" t="n">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>0.53%</t>
+          <t>0.49%</t>
         </is>
       </c>
       <c r="J64" t="n">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>-0.02%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J65" t="n">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>-0.33%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J66" t="n">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>0.76%</t>
+          <t>0.55%</t>
         </is>
       </c>
       <c r="J67" t="n">
@@ -3964,7 +3964,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>-0.94%</t>
+          <t>-0.88%</t>
         </is>
       </c>
       <c r="J68" t="n">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>-0.45%</t>
+          <t>-1.61%</t>
         </is>
       </c>
       <c r="J69" t="n">
@@ -4068,7 +4068,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>-2.56%</t>
+          <t>-2.82%</t>
         </is>
       </c>
       <c r="J70" t="n">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>-0.97%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J71" t="n">
@@ -4172,7 +4172,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>-1.27%</t>
+          <t>-1.31%</t>
         </is>
       </c>
       <c r="J72" t="n">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>-1.41%</t>
+          <t>-1.49%</t>
         </is>
       </c>
       <c r="J73" t="n">
@@ -4276,7 +4276,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>-0.38%</t>
+          <t>-0.37%</t>
         </is>
       </c>
       <c r="J74" t="n">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>-1.92%</t>
+          <t>-1.97%</t>
         </is>
       </c>
       <c r="J75" t="n">
@@ -4380,7 +4380,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>-0.84%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J76" t="n">
@@ -4432,7 +4432,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>0.41%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J77" t="n">
@@ -4484,7 +4484,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>0.83%</t>
+          <t>0.92%</t>
         </is>
       </c>
       <c r="J78" t="n">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>0.95%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="J79" t="n">
@@ -4588,7 +4588,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J80" t="n">
@@ -4640,7 +4640,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>0.12%</t>
+          <t>1.22%</t>
         </is>
       </c>
       <c r="J81" t="n">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>0.07%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J82" t="n">
@@ -4744,7 +4744,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>-0.7%</t>
+          <t>-1.03%</t>
         </is>
       </c>
       <c r="J83" t="n">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>-1.05%</t>
+          <t>-1.04%</t>
         </is>
       </c>
       <c r="J84" t="n">
@@ -4848,7 +4848,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>0.37%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J85" t="n">
@@ -4900,7 +4900,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>-1.72%</t>
+          <t>-1.7%</t>
         </is>
       </c>
       <c r="J86" t="n">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J87" t="n">
@@ -5004,7 +5004,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>-0.73%</t>
+          <t>-0.77%</t>
         </is>
       </c>
       <c r="J88" t="n">
@@ -5056,7 +5056,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>-1.4%</t>
+          <t>-1.25%</t>
         </is>
       </c>
       <c r="J89" t="n">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>-0.64%</t>
+          <t>-0.94%</t>
         </is>
       </c>
       <c r="J90" t="n">
@@ -5160,7 +5160,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>-2.14%</t>
+          <t>-2.0%</t>
         </is>
       </c>
       <c r="J91" t="n">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>1.09%</t>
+          <t>0.99%</t>
         </is>
       </c>
       <c r="J92" t="n">
@@ -5264,7 +5264,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>-0.27%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J93" t="n">
@@ -5316,7 +5316,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>-0.63%</t>
+          <t>-0.85%</t>
         </is>
       </c>
       <c r="J94" t="n">
@@ -5368,7 +5368,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>-0.16%</t>
+          <t>-1.33%</t>
         </is>
       </c>
       <c r="J95" t="n">
@@ -5420,7 +5420,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>-1.0%</t>
+          <t>-2.0%</t>
         </is>
       </c>
       <c r="J96" t="n">
@@ -5472,7 +5472,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>-0.24%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J97" t="n">
@@ -5524,7 +5524,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>0.23%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J98" t="n">
@@ -5576,7 +5576,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>0.74%</t>
+          <t>0.53%</t>
         </is>
       </c>
       <c r="J99" t="n">
@@ -5628,7 +5628,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>-0.34%</t>
+          <t>-0.35%</t>
         </is>
       </c>
       <c r="J100" t="n">
@@ -5680,7 +5680,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>0.74%</t>
+          <t>1.3%</t>
         </is>
       </c>
       <c r="J101" t="n">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>-0.55%</t>
+          <t>-0.51%</t>
         </is>
       </c>
       <c r="J102" t="n">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>-0.04%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J103" t="n">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>0.02%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J104" t="n">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.34%</t>
         </is>
       </c>
       <c r="J105" t="n">
@@ -5940,7 +5940,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.36%</t>
         </is>
       </c>
       <c r="J106" t="n">
@@ -5992,7 +5992,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>-0.52%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J107" t="n">
@@ -6044,7 +6044,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>0.67%</t>
+          <t>0.75%</t>
         </is>
       </c>
       <c r="J108" t="n">
@@ -6096,7 +6096,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>-0.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J109" t="n">
@@ -6148,7 +6148,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>-2.5%</t>
+          <t>-2.54%</t>
         </is>
       </c>
       <c r="J110" t="n">
@@ -6200,7 +6200,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>1.06%</t>
+          <t>1.43%</t>
         </is>
       </c>
       <c r="J111" t="n">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>-0.56%</t>
+          <t>-0.77%</t>
         </is>
       </c>
       <c r="J112" t="n">
@@ -6304,7 +6304,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>1.48%</t>
+          <t>1.44%</t>
         </is>
       </c>
       <c r="J113" t="n">
@@ -6356,7 +6356,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>-0.7%</t>
+          <t>-0.74%</t>
         </is>
       </c>
       <c r="J114" t="n">
@@ -6408,7 +6408,7 @@
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>-0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J115" t="n">
@@ -6460,7 +6460,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>-1.49%</t>
+          <t>-1.89%</t>
         </is>
       </c>
       <c r="J116" t="n">
@@ -6512,7 +6512,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>0.36%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J117" t="n">
@@ -6564,7 +6564,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>0.58%</t>
+          <t>0.74%</t>
         </is>
       </c>
       <c r="J118" t="n">
@@ -6616,7 +6616,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>0.96%</t>
+          <t>0.85%</t>
         </is>
       </c>
       <c r="J119" t="n">
@@ -6668,7 +6668,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>0.32%</t>
+          <t>0.26%</t>
         </is>
       </c>
       <c r="J120" t="n">
@@ -6720,7 +6720,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>1.23%</t>
+          <t>1.14%</t>
         </is>
       </c>
       <c r="J121" t="n">
@@ -6772,7 +6772,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>-1.57%</t>
+          <t>-1.48%</t>
         </is>
       </c>
       <c r="J122" t="n">
@@ -6824,7 +6824,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>-0.92%</t>
+          <t>-0.82%</t>
         </is>
       </c>
       <c r="J123" t="n">
@@ -6876,7 +6876,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>-0.47%</t>
+          <t>-0.71%</t>
         </is>
       </c>
       <c r="J124" t="n">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J125" t="n">
@@ -6980,7 +6980,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>0.68%</t>
+          <t>0.65%</t>
         </is>
       </c>
       <c r="J126" t="n">
@@ -7032,7 +7032,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>-0.25%</t>
+          <t>-0.42%</t>
         </is>
       </c>
       <c r="J127" t="n">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>0.08%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J128" t="n">
@@ -7136,7 +7136,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>-2.76%</t>
+          <t>-2.22%</t>
         </is>
       </c>
       <c r="J129" t="n">
@@ -7188,7 +7188,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>0.44%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J130" t="n">
@@ -7240,7 +7240,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>0.08%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J131" t="n">
@@ -7292,7 +7292,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>0.29%</t>
+          <t>0.45%</t>
         </is>
       </c>
       <c r="J132" t="n">
@@ -7344,7 +7344,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>0.68%</t>
+          <t>1.3%</t>
         </is>
       </c>
       <c r="J133" t="n">
@@ -7396,7 +7396,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>-0.92%</t>
+          <t>-1.44%</t>
         </is>
       </c>
       <c r="J134" t="n">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>2.37%</t>
+          <t>2.24%</t>
         </is>
       </c>
       <c r="J135" t="n">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>0.44%</t>
+          <t>0.64%</t>
         </is>
       </c>
       <c r="J137" t="n">
@@ -7604,7 +7604,7 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>-0.92%</t>
+          <t>-0.66%</t>
         </is>
       </c>
       <c r="J138" t="n">
@@ -7656,7 +7656,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>-0.87%</t>
+          <t>-0.73%</t>
         </is>
       </c>
       <c r="J139" t="n">
@@ -7708,7 +7708,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>0.92%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="J140" t="n">
@@ -7760,7 +7760,7 @@
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>-0.53%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J141" t="n">
@@ -7812,7 +7812,7 @@
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>-1.66%</t>
+          <t>-1.72%</t>
         </is>
       </c>
       <c r="J142" t="n">
@@ -7864,7 +7864,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>-0.35%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J143" t="n">
@@ -7916,7 +7916,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>-1.06%</t>
+          <t>-1.87%</t>
         </is>
       </c>
       <c r="J144" t="n">
@@ -8020,7 +8020,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>-0.27%</t>
+          <t>-0.37%</t>
         </is>
       </c>
       <c r="J146" t="n">
@@ -8072,7 +8072,7 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>-0.01%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J147" t="n">
@@ -8124,7 +8124,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>0.58%</t>
+          <t>0.67%</t>
         </is>
       </c>
       <c r="J148" t="n">
@@ -8176,7 +8176,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>-0.31%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J149" t="n">
@@ -8228,7 +8228,7 @@
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>-0.94%</t>
+          <t>-0.88%</t>
         </is>
       </c>
       <c r="J150" t="n">
@@ -8280,7 +8280,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>0.75%</t>
+          <t>0.84%</t>
         </is>
       </c>
       <c r="J151" t="n">
@@ -8332,7 +8332,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>0.61%</t>
+          <t>0.52%</t>
         </is>
       </c>
       <c r="J152" t="n">
@@ -8384,7 +8384,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>-0.24%</t>
+          <t>-0.22%</t>
         </is>
       </c>
       <c r="J153" t="n">
@@ -8436,7 +8436,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>0.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J154" t="n">
@@ -8488,7 +8488,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>0.28%</t>
+          <t>1.05%</t>
         </is>
       </c>
       <c r="J155" t="n">
@@ -8540,7 +8540,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>-0.13%</t>
+          <t>-0.2%</t>
         </is>
       </c>
       <c r="J156" t="n">
@@ -8592,7 +8592,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>0.42%</t>
         </is>
       </c>
       <c r="J157" t="n">
@@ -8644,7 +8644,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>-1.13%</t>
+          <t>-1.38%</t>
         </is>
       </c>
       <c r="J158" t="n">
@@ -8696,7 +8696,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>-0.6%</t>
+          <t>-0.87%</t>
         </is>
       </c>
       <c r="J159" t="n">
@@ -8748,7 +8748,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>-0.59%</t>
+          <t>-0.43%</t>
         </is>
       </c>
       <c r="J160" t="n">
@@ -8800,7 +8800,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>1.07%</t>
+          <t>0.96%</t>
         </is>
       </c>
       <c r="J161" t="n">
@@ -8852,7 +8852,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>-1.21%</t>
+          <t>-1.69%</t>
         </is>
       </c>
       <c r="J162" t="n">
@@ -8904,7 +8904,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>0.43%</t>
+          <t>0.62%</t>
         </is>
       </c>
       <c r="J163" t="n">
@@ -8956,7 +8956,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>-0.69%</t>
+          <t>-0.42%</t>
         </is>
       </c>
       <c r="J164" t="n">
@@ -9008,7 +9008,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>-0.78%</t>
+          <t>-1.39%</t>
         </is>
       </c>
       <c r="J165" t="n">
@@ -9060,7 +9060,7 @@
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>-0.38%</t>
+          <t>-0.34%</t>
         </is>
       </c>
       <c r="J166" t="n">
@@ -9112,7 +9112,7 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>-0.42%</t>
+          <t>-1.04%</t>
         </is>
       </c>
       <c r="J167" t="n">
@@ -9164,7 +9164,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>-2.52%</t>
+          <t>-2.17%</t>
         </is>
       </c>
       <c r="J168" t="n">
@@ -9216,7 +9216,7 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>-0.95%</t>
+          <t>-1.33%</t>
         </is>
       </c>
       <c r="J169" t="n">
@@ -9268,7 +9268,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>-0.08%</t>
+          <t>-0.77%</t>
         </is>
       </c>
       <c r="J170" t="n">
@@ -9320,7 +9320,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>-1.39%</t>
+          <t>-1.09%</t>
         </is>
       </c>
       <c r="J171" t="n">
@@ -9372,7 +9372,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>1.32%</t>
+          <t>1.34%</t>
         </is>
       </c>
       <c r="J172" t="n">
@@ -9424,7 +9424,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>-0.35%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J173" t="n">
@@ -9476,7 +9476,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>-0.95%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J174" t="n">
@@ -9528,7 +9528,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>-1.01%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J175" t="n">
@@ -9580,7 +9580,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>-2.22%</t>
+          <t>-1.52%</t>
         </is>
       </c>
       <c r="J176" t="n">
@@ -9632,7 +9632,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>-0.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J177" t="n">
@@ -9684,7 +9684,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>-1.18%</t>
+          <t>-1.75%</t>
         </is>
       </c>
       <c r="J178" t="n">
@@ -9736,7 +9736,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>0.41%</t>
+          <t>1.25%</t>
         </is>
       </c>
       <c r="J179" t="n">
@@ -9788,7 +9788,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>0.12%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J180" t="n">
@@ -9840,7 +9840,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>1.23%</t>
+          <t>1.65%</t>
         </is>
       </c>
       <c r="J181" t="n">
@@ -9892,7 +9892,7 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>-0.98%</t>
+          <t>-1.33%</t>
         </is>
       </c>
       <c r="J182" t="n">
@@ -9944,7 +9944,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>-1.3%</t>
+          <t>-2.04%</t>
         </is>
       </c>
       <c r="J183" t="n">
@@ -9996,7 +9996,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J184" t="n">
@@ -10048,7 +10048,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>-0.07%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J185" t="n">
@@ -10100,7 +10100,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>0.55%</t>
+          <t>0.56%</t>
         </is>
       </c>
       <c r="J186" t="n">
@@ -10152,7 +10152,7 @@
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>-0.02%</t>
+          <t>-0.04%</t>
         </is>
       </c>
       <c r="J187" t="n">
@@ -10204,7 +10204,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>-0.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J188" t="n">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>-2.56%</t>
+          <t>-2.63%</t>
         </is>
       </c>
       <c r="J189" t="n">
@@ -10308,7 +10308,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>0.87%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J190" t="n">
@@ -10360,7 +10360,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>0.08%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J191" t="n">
@@ -10412,7 +10412,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>1.07%</t>
+          <t>0.77%</t>
         </is>
       </c>
       <c r="J192" t="n">
@@ -10464,7 +10464,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>-0.28%</t>
+          <t>-0.37%</t>
         </is>
       </c>
       <c r="J193" t="n">
@@ -10516,7 +10516,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>-0.97%</t>
+          <t>-1.36%</t>
         </is>
       </c>
       <c r="J194" t="n">
@@ -10568,7 +10568,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>-1.42%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J195" t="n">
@@ -10620,7 +10620,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>0.53%</t>
+          <t>0.42%</t>
         </is>
       </c>
       <c r="J196" t="n">
@@ -10672,7 +10672,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>-0.63%</t>
+          <t>-0.71%</t>
         </is>
       </c>
       <c r="J197" t="n">
@@ -10724,7 +10724,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>-2.77%</t>
+          <t>-1.75%</t>
         </is>
       </c>
       <c r="J198" t="n">
@@ -10776,7 +10776,7 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>-0.62%</t>
+          <t>-1.22%</t>
         </is>
       </c>
       <c r="J199" t="n">
@@ -10828,7 +10828,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>-1.0%</t>
+          <t>-1.01%</t>
         </is>
       </c>
       <c r="J200" t="n">
@@ -10880,7 +10880,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>-0.85%</t>
+          <t>-0.57%</t>
         </is>
       </c>
       <c r="J201" t="n">
@@ -10932,7 +10932,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>-0.94%</t>
+          <t>-2.86%</t>
         </is>
       </c>
       <c r="J202" t="n">
@@ -10984,7 +10984,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.19%</t>
         </is>
       </c>
       <c r="J203" t="n">
@@ -11036,7 +11036,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>-0.11%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J204" t="n">
@@ -11088,7 +11088,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>-1.29%</t>
+          <t>-1.34%</t>
         </is>
       </c>
       <c r="J205" t="n">
@@ -11140,7 +11140,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>0.62%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="J206" t="n">
@@ -11192,7 +11192,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>-0.76%</t>
+          <t>-0.88%</t>
         </is>
       </c>
       <c r="J207" t="n">
@@ -11244,7 +11244,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>-0.14%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J208" t="n">
@@ -11296,7 +11296,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>-1.55%</t>
+          <t>-1.75%</t>
         </is>
       </c>
       <c r="J209" t="n">
@@ -11348,7 +11348,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>0.68%</t>
+          <t>0.84%</t>
         </is>
       </c>
       <c r="J210" t="n">
@@ -11400,7 +11400,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>-1.11%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J211" t="n">
@@ -11452,7 +11452,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>-0.43%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J212" t="n">
@@ -11504,7 +11504,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>-0.84%</t>
+          <t>-0.5%</t>
         </is>
       </c>
       <c r="J213" t="n">
@@ -11556,7 +11556,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>-0.04%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J214" t="n">
@@ -11608,7 +11608,7 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J215" t="n">
@@ -11660,7 +11660,7 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>0.73%</t>
+          <t>0.48%</t>
         </is>
       </c>
       <c r="J216" t="n">
@@ -11712,7 +11712,7 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>-0.84%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J217" t="n">
@@ -11764,7 +11764,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>-1.19%</t>
+          <t>-1.92%</t>
         </is>
       </c>
       <c r="J218" t="n">
@@ -11816,7 +11816,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>-1.01%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J219" t="n">
@@ -11868,7 +11868,7 @@
       </c>
       <c r="I220" t="inlineStr">
         <is>
-          <t>-4.06%</t>
+          <t>-4.0%</t>
         </is>
       </c>
       <c r="J220" t="n">
@@ -11920,7 +11920,7 @@
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>1.56%</t>
+          <t>1.54%</t>
         </is>
       </c>
       <c r="J221" t="n">
@@ -11972,7 +11972,7 @@
       </c>
       <c r="I222" t="inlineStr">
         <is>
-          <t>-1.54%</t>
+          <t>-1.56%</t>
         </is>
       </c>
       <c r="J222" t="n">
@@ -12024,7 +12024,7 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>-0.18%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J223" t="n">
@@ -12076,7 +12076,7 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>-0.4%</t>
+          <t>-0.27%</t>
         </is>
       </c>
       <c r="J224" t="n">
@@ -12128,7 +12128,7 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>-0.46%</t>
+          <t>-1.32%</t>
         </is>
       </c>
       <c r="J225" t="n">
@@ -12180,7 +12180,7 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>-0.91%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J226" t="n">
@@ -12232,7 +12232,7 @@
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>-0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J227" t="n">
@@ -12284,7 +12284,7 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>-0.07%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J228" t="n">
@@ -12336,7 +12336,7 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>-0.83%</t>
+          <t>-0.96%</t>
         </is>
       </c>
       <c r="J229" t="n">
@@ -12388,7 +12388,7 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>-1.08%</t>
+          <t>-0.72%</t>
         </is>
       </c>
       <c r="J230" t="n">
@@ -12440,7 +12440,7 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>0.15%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J231" t="n">
@@ -12492,7 +12492,7 @@
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>-1.51%</t>
+          <t>-1.37%</t>
         </is>
       </c>
       <c r="J232" t="n">
@@ -12544,7 +12544,7 @@
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>-0.74%</t>
+          <t>-1.11%</t>
         </is>
       </c>
       <c r="J233" t="n">
@@ -12596,7 +12596,7 @@
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>0.46%</t>
+          <t>0.78%</t>
         </is>
       </c>
       <c r="J234" t="n">
@@ -12648,7 +12648,7 @@
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J235" t="n">
@@ -12700,7 +12700,7 @@
       </c>
       <c r="I236" t="inlineStr">
         <is>
-          <t>-0.25%</t>
+          <t>-0.72%</t>
         </is>
       </c>
       <c r="J236" t="n">
@@ -12752,7 +12752,7 @@
       </c>
       <c r="I237" t="inlineStr">
         <is>
-          <t>0.25%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="J237" t="n">
@@ -12804,7 +12804,7 @@
       </c>
       <c r="I238" t="inlineStr">
         <is>
-          <t>-1.46%</t>
+          <t>-2.35%</t>
         </is>
       </c>
       <c r="J238" t="n">
@@ -12856,7 +12856,7 @@
       </c>
       <c r="I239" t="inlineStr">
         <is>
-          <t>-0.63%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J239" t="n">
@@ -12908,7 +12908,7 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>-0.31%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J240" t="n">
@@ -12960,7 +12960,7 @@
       </c>
       <c r="I241" t="inlineStr">
         <is>
-          <t>0.37%</t>
+          <t>1.69%</t>
         </is>
       </c>
       <c r="J241" t="n">
@@ -13012,7 +13012,7 @@
       </c>
       <c r="I242" t="inlineStr">
         <is>
-          <t>1.03%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="J242" t="n">
@@ -13064,7 +13064,7 @@
       </c>
       <c r="I243" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J243" t="n">
@@ -13116,7 +13116,7 @@
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>0.18%</t>
+          <t>0.33%</t>
         </is>
       </c>
       <c r="J244" t="n">
@@ -13168,7 +13168,7 @@
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>-0.82%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J245" t="n">
@@ -13220,7 +13220,7 @@
       </c>
       <c r="I246" t="inlineStr">
         <is>
-          <t>0.74%</t>
+          <t>0.85%</t>
         </is>
       </c>
       <c r="J246" t="n">
@@ -13272,7 +13272,7 @@
       </c>
       <c r="I247" t="inlineStr">
         <is>
-          <t>0.78%</t>
+          <t>1.64%</t>
         </is>
       </c>
       <c r="J247" t="n">
@@ -13324,7 +13324,7 @@
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>-0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J248" t="n">
@@ -13376,7 +13376,7 @@
       </c>
       <c r="I249" t="inlineStr">
         <is>
-          <t>-2.66%</t>
+          <t>-2.86%</t>
         </is>
       </c>
       <c r="J249" t="n">
@@ -13428,7 +13428,7 @@
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>0.08%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J250" t="n">
@@ -13480,7 +13480,7 @@
       </c>
       <c r="I251" t="inlineStr">
         <is>
-          <t>0.64%</t>
+          <t>2.17%</t>
         </is>
       </c>
       <c r="J251" t="n">
@@ -13532,7 +13532,7 @@
       </c>
       <c r="I252" t="inlineStr">
         <is>
-          <t>-0.77%</t>
+          <t>-0.78%</t>
         </is>
       </c>
       <c r="J252" t="n">
@@ -13584,7 +13584,7 @@
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>-0.61%</t>
+          <t>-0.66%</t>
         </is>
       </c>
       <c r="J253" t="n">
@@ -13636,7 +13636,7 @@
       </c>
       <c r="I254" t="inlineStr">
         <is>
-          <t>2.61%</t>
+          <t>2.27%</t>
         </is>
       </c>
       <c r="J254" t="n">
@@ -13688,7 +13688,7 @@
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>-0.52%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J255" t="n">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>-1.23%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J256" t="n">
@@ -13792,7 +13792,7 @@
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>-0.76%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J257" t="n">
@@ -13844,7 +13844,7 @@
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>0.69%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J258" t="n">
@@ -13896,7 +13896,7 @@
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>-0.07%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J259" t="n">
@@ -13948,7 +13948,7 @@
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>-0.07%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J260" t="n">
@@ -14000,7 +14000,7 @@
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>-0.12%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J261" t="n">
@@ -14052,7 +14052,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>-1.29%</t>
+          <t>-0.82%</t>
         </is>
       </c>
       <c r="J262" t="n">
@@ -14104,7 +14104,7 @@
       </c>
       <c r="I263" t="inlineStr">
         <is>
-          <t>-0.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J263" t="n">
@@ -14156,7 +14156,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>0.18%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J264" t="n">
@@ -14208,7 +14208,7 @@
       </c>
       <c r="I265" t="inlineStr">
         <is>
-          <t>-0.87%</t>
+          <t>-0.8%</t>
         </is>
       </c>
       <c r="J265" t="n">
@@ -14260,7 +14260,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>-0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J266" t="n">
@@ -14312,7 +14312,7 @@
       </c>
       <c r="I267" t="inlineStr">
         <is>
-          <t>0.12%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="J267" t="n">
@@ -14364,7 +14364,7 @@
       </c>
       <c r="I268" t="inlineStr">
         <is>
-          <t>-0.49%</t>
+          <t>-1.33%</t>
         </is>
       </c>
       <c r="J268" t="n">
@@ -14416,7 +14416,7 @@
       </c>
       <c r="I269" t="inlineStr">
         <is>
-          <t>-0.58%</t>
+          <t>-0.89%</t>
         </is>
       </c>
       <c r="J269" t="n">
@@ -14468,7 +14468,7 @@
       </c>
       <c r="I270" t="inlineStr">
         <is>
-          <t>-1.37%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J270" t="n">
@@ -14520,7 +14520,7 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>-0.84%</t>
+          <t>-0.89%</t>
         </is>
       </c>
       <c r="J271" t="n">
@@ -14572,7 +14572,7 @@
       </c>
       <c r="I272" t="inlineStr">
         <is>
-          <t>-2.84%</t>
+          <t>-8.33%</t>
         </is>
       </c>
       <c r="J272" t="n">
@@ -14624,7 +14624,7 @@
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>-0.72%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J273" t="n">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>-0.72%</t>
+          <t>-0.76%</t>
         </is>
       </c>
       <c r="J274" t="n">
@@ -14728,7 +14728,7 @@
       </c>
       <c r="I275" t="inlineStr">
         <is>
-          <t>1.21%</t>
+          <t>1.15%</t>
         </is>
       </c>
       <c r="J275" t="n">
@@ -14780,7 +14780,7 @@
       </c>
       <c r="I276" t="inlineStr">
         <is>
-          <t>0.78%</t>
+          <t>1.75%</t>
         </is>
       </c>
       <c r="J276" t="n">
@@ -14832,7 +14832,7 @@
       </c>
       <c r="I277" t="inlineStr">
         <is>
-          <t>-0.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J277" t="n">
@@ -14884,7 +14884,7 @@
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>-0.32%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J278" t="n">
@@ -14936,7 +14936,7 @@
       </c>
       <c r="I279" t="inlineStr">
         <is>
-          <t>-0.57%</t>
+          <t>-0.64%</t>
         </is>
       </c>
       <c r="J279" t="n">
@@ -14988,7 +14988,7 @@
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>0.08%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J280" t="n">
@@ -15040,7 +15040,7 @@
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>-3.39%</t>
+          <t>-3.08%</t>
         </is>
       </c>
       <c r="J281" t="n">
@@ -15092,7 +15092,7 @@
       </c>
       <c r="I282" t="inlineStr">
         <is>
-          <t>-1.23%</t>
+          <t>-1.25%</t>
         </is>
       </c>
       <c r="J282" t="n">
@@ -15144,7 +15144,7 @@
       </c>
       <c r="I283" t="inlineStr">
         <is>
-          <t>0.98%</t>
+          <t>0.53%</t>
         </is>
       </c>
       <c r="J283" t="n">
@@ -15196,7 +15196,7 @@
       </c>
       <c r="I284" t="inlineStr">
         <is>
-          <t>-0.47%</t>
+          <t>-1.43%</t>
         </is>
       </c>
       <c r="J284" t="n">
@@ -15248,7 +15248,7 @@
       </c>
       <c r="I285" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J285" t="n">
@@ -15300,7 +15300,7 @@
       </c>
       <c r="I286" t="inlineStr">
         <is>
-          <t>0.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J286" t="n">
@@ -15352,7 +15352,7 @@
       </c>
       <c r="I287" t="inlineStr">
         <is>
-          <t>-0.87%</t>
+          <t>-0.81%</t>
         </is>
       </c>
       <c r="J287" t="n">
@@ -15404,7 +15404,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>-1.95%</t>
+          <t>-2.38%</t>
         </is>
       </c>
       <c r="J288" t="n">
@@ -15456,7 +15456,7 @@
       </c>
       <c r="I289" t="inlineStr">
         <is>
-          <t>-1.18%</t>
+          <t>-1.11%</t>
         </is>
       </c>
       <c r="J289" t="n">
@@ -15508,7 +15508,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>-0.54%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J290" t="n">
@@ -15560,7 +15560,7 @@
       </c>
       <c r="I291" t="inlineStr">
         <is>
-          <t>0.46%</t>
+          <t>0.34%</t>
         </is>
       </c>
       <c r="J291" t="n">
@@ -15664,7 +15664,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>-0.76%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J293" t="n">
@@ -15716,7 +15716,7 @@
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>-0.73%</t>
+          <t>-0.76%</t>
         </is>
       </c>
       <c r="J294" t="n">
@@ -15768,7 +15768,7 @@
       </c>
       <c r="I295" t="inlineStr">
         <is>
-          <t>-0.17%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J295" t="n">
@@ -15820,7 +15820,7 @@
       </c>
       <c r="I296" t="inlineStr">
         <is>
-          <t>0.54%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J296" t="n">
@@ -15872,7 +15872,7 @@
       </c>
       <c r="I297" t="inlineStr">
         <is>
-          <t>-0.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J297" t="n">
@@ -15924,7 +15924,7 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>-0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J298" t="n">
@@ -15976,7 +15976,7 @@
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>-0.96%</t>
+          <t>-1.14%</t>
         </is>
       </c>
       <c r="J299" t="n">
@@ -16028,7 +16028,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>0.17%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J300" t="n">
@@ -16132,7 +16132,7 @@
       </c>
       <c r="I302" t="inlineStr">
         <is>
-          <t>0.22%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J302" t="n">
@@ -16184,7 +16184,7 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>0.81%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="J303" t="n">
@@ -16236,7 +16236,7 @@
       </c>
       <c r="I304" t="inlineStr">
         <is>
-          <t>-0.92%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J304" t="n">
@@ -16288,7 +16288,7 @@
       </c>
       <c r="I305" t="inlineStr">
         <is>
-          <t>-0.6%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J305" t="n">
@@ -16340,7 +16340,7 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>0.44%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J306" t="n">
@@ -16392,7 +16392,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>-1.04%</t>
+          <t>-1.28%</t>
         </is>
       </c>
       <c r="J307" t="n">
@@ -16444,7 +16444,7 @@
       </c>
       <c r="I308" t="inlineStr">
         <is>
-          <t>-0.5%</t>
+          <t>-0.41%</t>
         </is>
       </c>
       <c r="J308" t="n">
@@ -16496,7 +16496,7 @@
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J309" t="n">
@@ -16548,7 +16548,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>-0.96%</t>
+          <t>-0.92%</t>
         </is>
       </c>
       <c r="J310" t="n">
@@ -16600,7 +16600,7 @@
       </c>
       <c r="I311" t="inlineStr">
         <is>
-          <t>0.89%</t>
+          <t>0.91%</t>
         </is>
       </c>
       <c r="J311" t="n">
@@ -16652,7 +16652,7 @@
       </c>
       <c r="I312" t="inlineStr">
         <is>
-          <t>0.88%</t>
+          <t>0.51%</t>
         </is>
       </c>
       <c r="J312" t="n">
@@ -16704,7 +16704,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t>0.68%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J313" t="n">
@@ -16756,7 +16756,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>-3.7%</t>
+          <t>-3.52%</t>
         </is>
       </c>
       <c r="J314" t="n">
@@ -16808,7 +16808,7 @@
       </c>
       <c r="I315" t="inlineStr">
         <is>
-          <t>-0.37%</t>
+          <t>-0.91%</t>
         </is>
       </c>
       <c r="J315" t="n">
@@ -16860,7 +16860,7 @@
       </c>
       <c r="I316" t="inlineStr">
         <is>
-          <t>-1.5%</t>
+          <t>-1.53%</t>
         </is>
       </c>
       <c r="J316" t="n">
@@ -16912,7 +16912,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>2.44%</t>
         </is>
       </c>
       <c r="J317" t="n">
@@ -16964,7 +16964,7 @@
       </c>
       <c r="I318" t="inlineStr">
         <is>
-          <t>-0.27%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J318" t="n">
@@ -17016,7 +17016,7 @@
       </c>
       <c r="I319" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J319" t="n">
@@ -17068,7 +17068,7 @@
       </c>
       <c r="I320" t="inlineStr">
         <is>
-          <t>0.38%</t>
+          <t>1.92%</t>
         </is>
       </c>
       <c r="J320" t="n">
@@ -17120,7 +17120,7 @@
       </c>
       <c r="I321" t="inlineStr">
         <is>
-          <t>-0.3%</t>
+          <t>-0.29%</t>
         </is>
       </c>
       <c r="J321" t="n">
@@ -17172,7 +17172,7 @@
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>0.45%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J322" t="n">
@@ -17224,7 +17224,7 @@
       </c>
       <c r="I323" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J323" t="n">
@@ -17276,7 +17276,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>-1.11%</t>
+          <t>-4.0%</t>
         </is>
       </c>
       <c r="J324" t="n">
@@ -17328,7 +17328,7 @@
       </c>
       <c r="I325" t="inlineStr">
         <is>
-          <t>0.58%</t>
+          <t>1.09%</t>
         </is>
       </c>
       <c r="J325" t="n">
@@ -17380,7 +17380,7 @@
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>0.52%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J326" t="n">
@@ -17432,7 +17432,7 @@
       </c>
       <c r="I327" t="inlineStr">
         <is>
-          <t>0.23%</t>
+          <t>0.27%</t>
         </is>
       </c>
       <c r="J327" t="n">
@@ -17484,7 +17484,7 @@
       </c>
       <c r="I328" t="inlineStr">
         <is>
-          <t>1.08%</t>
+          <t>0.94%</t>
         </is>
       </c>
       <c r="J328" t="n">
@@ -17536,7 +17536,7 @@
       </c>
       <c r="I329" t="inlineStr">
         <is>
-          <t>-0.62%</t>
+          <t>-0.66%</t>
         </is>
       </c>
       <c r="J329" t="n">
@@ -17588,7 +17588,7 @@
       </c>
       <c r="I330" t="inlineStr">
         <is>
-          <t>-0.49%</t>
+          <t>-2.7%</t>
         </is>
       </c>
       <c r="J330" t="n">
@@ -17640,7 +17640,7 @@
       </c>
       <c r="I331" t="inlineStr">
         <is>
-          <t>-0.35%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J331" t="n">
@@ -17692,7 +17692,7 @@
       </c>
       <c r="I332" t="inlineStr">
         <is>
-          <t>-1.03%</t>
+          <t>-0.96%</t>
         </is>
       </c>
       <c r="J332" t="n">
@@ -17744,7 +17744,7 @@
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>0.61%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J333" t="n">
@@ -17796,7 +17796,7 @@
       </c>
       <c r="I334" t="inlineStr">
         <is>
-          <t>1.26%</t>
+          <t>1.37%</t>
         </is>
       </c>
       <c r="J334" t="n">
@@ -17848,7 +17848,7 @@
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t>-2.23%</t>
+          <t>-2.27%</t>
         </is>
       </c>
       <c r="J335" t="n">
@@ -17900,7 +17900,7 @@
       </c>
       <c r="I336" t="inlineStr">
         <is>
-          <t>0.25%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J336" t="n">
@@ -17952,7 +17952,7 @@
       </c>
       <c r="I337" t="inlineStr">
         <is>
-          <t>-2.34%</t>
+          <t>-2.46%</t>
         </is>
       </c>
       <c r="J337" t="n">
@@ -18004,7 +18004,7 @@
       </c>
       <c r="I338" t="inlineStr">
         <is>
-          <t>1.37%</t>
+          <t>1.43%</t>
         </is>
       </c>
       <c r="J338" t="n">
@@ -18056,7 +18056,7 @@
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>-1.24%</t>
+          <t>-1.25%</t>
         </is>
       </c>
       <c r="J339" t="n">
@@ -18108,7 +18108,7 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>2.46%</t>
+          <t>2.45%</t>
         </is>
       </c>
       <c r="J340" t="n">
@@ -18160,7 +18160,7 @@
       </c>
       <c r="I341" t="inlineStr">
         <is>
-          <t>-0.25%</t>
+          <t>-0.47%</t>
         </is>
       </c>
       <c r="J341" t="n">
@@ -18212,7 +18212,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>-0.29%</t>
+          <t>-0.36%</t>
         </is>
       </c>
       <c r="J342" t="n">
@@ -18264,7 +18264,7 @@
       </c>
       <c r="I343" t="inlineStr">
         <is>
-          <t>2.82%</t>
+          <t>2.76%</t>
         </is>
       </c>
       <c r="J343" t="n">
@@ -18316,7 +18316,7 @@
       </c>
       <c r="I344" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J344" t="n">
@@ -18368,7 +18368,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>2.08%</t>
+          <t>1.27%</t>
         </is>
       </c>
       <c r="J345" t="n">
@@ -18420,7 +18420,7 @@
       </c>
       <c r="I346" t="inlineStr">
         <is>
-          <t>-0.97%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J346" t="n">
@@ -18472,7 +18472,7 @@
       </c>
       <c r="I347" t="inlineStr">
         <is>
-          <t>-0.33%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J347" t="n">
@@ -18524,7 +18524,7 @@
       </c>
       <c r="I348" t="inlineStr">
         <is>
-          <t>-4.96%</t>
+          <t>-4.69%</t>
         </is>
       </c>
       <c r="J348" t="n">
@@ -18628,7 +18628,7 @@
       </c>
       <c r="I350" t="inlineStr">
         <is>
-          <t>0.69%</t>
+          <t>0.72%</t>
         </is>
       </c>
       <c r="J350" t="n">
@@ -18680,7 +18680,7 @@
       </c>
       <c r="I351" t="inlineStr">
         <is>
-          <t>-1.34%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J351" t="n">
@@ -18732,7 +18732,7 @@
       </c>
       <c r="I352" t="inlineStr">
         <is>
-          <t>-1.12%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J352" t="n">
@@ -18784,7 +18784,7 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>-1.25%</t>
+          <t>-2.3%</t>
         </is>
       </c>
       <c r="J353" t="n">
@@ -18836,7 +18836,7 @@
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>0.88%</t>
+          <t>0.79%</t>
         </is>
       </c>
       <c r="J354" t="n">
@@ -18888,7 +18888,7 @@
       </c>
       <c r="I355" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.62%</t>
         </is>
       </c>
       <c r="J355" t="n">
@@ -18940,7 +18940,7 @@
       </c>
       <c r="I356" t="inlineStr">
         <is>
-          <t>-1.21%</t>
+          <t>-1.39%</t>
         </is>
       </c>
       <c r="J356" t="n">
@@ -18992,7 +18992,7 @@
       </c>
       <c r="I357" t="inlineStr">
         <is>
-          <t>-0.49%</t>
+          <t>-0.9%</t>
         </is>
       </c>
       <c r="J357" t="n">
@@ -19044,7 +19044,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>-1.49%</t>
+          <t>-1.28%</t>
         </is>
       </c>
       <c r="J358" t="n">
@@ -19096,7 +19096,7 @@
       </c>
       <c r="I359" t="inlineStr">
         <is>
-          <t>1.02%</t>
+          <t>1.14%</t>
         </is>
       </c>
       <c r="J359" t="n">
@@ -19148,7 +19148,7 @@
       </c>
       <c r="I360" t="inlineStr">
         <is>
-          <t>-0.19%</t>
+          <t>-1.85%</t>
         </is>
       </c>
       <c r="J360" t="n">
@@ -19200,7 +19200,7 @@
       </c>
       <c r="I361" t="inlineStr">
         <is>
-          <t>-0.03%</t>
+          <t>-0.57%</t>
         </is>
       </c>
       <c r="J361" t="n">
@@ -19252,7 +19252,7 @@
       </c>
       <c r="I362" t="inlineStr">
         <is>
-          <t>1.12%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="J362" t="n">
@@ -19304,7 +19304,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t>-2.31%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J363" t="n">
@@ -19356,7 +19356,7 @@
       </c>
       <c r="I364" t="inlineStr">
         <is>
-          <t>-0.17%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J364" t="n">
@@ -19408,7 +19408,7 @@
       </c>
       <c r="I365" t="inlineStr">
         <is>
-          <t>0.14%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J365" t="n">
@@ -19460,7 +19460,7 @@
       </c>
       <c r="I366" t="inlineStr">
         <is>
-          <t>0.89%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J366" t="n">
@@ -19512,7 +19512,7 @@
       </c>
       <c r="I367" t="inlineStr">
         <is>
-          <t>-0.59%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J367" t="n">
@@ -19564,7 +19564,7 @@
       </c>
       <c r="I368" t="inlineStr">
         <is>
-          <t>-1.79%</t>
+          <t>-1.72%</t>
         </is>
       </c>
       <c r="J368" t="n">
@@ -19616,7 +19616,7 @@
       </c>
       <c r="I369" t="inlineStr">
         <is>
-          <t>0.61%</t>
+          <t>0.55%</t>
         </is>
       </c>
       <c r="J369" t="n">
@@ -19668,7 +19668,7 @@
       </c>
       <c r="I370" t="inlineStr">
         <is>
-          <t>0.39%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J370" t="n">
@@ -19720,7 +19720,7 @@
       </c>
       <c r="I371" t="inlineStr">
         <is>
-          <t>-0.7%</t>
+          <t>-0.89%</t>
         </is>
       </c>
       <c r="J371" t="n">
@@ -19772,7 +19772,7 @@
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>-2.84%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J372" t="n">
@@ -19824,7 +19824,7 @@
       </c>
       <c r="I373" t="inlineStr">
         <is>
-          <t>-0.34%</t>
+          <t>-0.6%</t>
         </is>
       </c>
       <c r="J373" t="n">
@@ -19876,7 +19876,7 @@
       </c>
       <c r="I374" t="inlineStr">
         <is>
-          <t>-0.26%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J374" t="n">
@@ -19928,7 +19928,7 @@
       </c>
       <c r="I375" t="inlineStr">
         <is>
-          <t>0.52%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J375" t="n">
@@ -19980,7 +19980,7 @@
       </c>
       <c r="I376" t="inlineStr">
         <is>
-          <t>1.78%</t>
+          <t>1.7%</t>
         </is>
       </c>
       <c r="J376" t="n">
@@ -20032,7 +20032,7 @@
       </c>
       <c r="I377" t="inlineStr">
         <is>
-          <t>-0.42%</t>
+          <t>-1.19%</t>
         </is>
       </c>
       <c r="J377" t="n">
@@ -20084,7 +20084,7 @@
       </c>
       <c r="I378" t="inlineStr">
         <is>
-          <t>0.01%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J378" t="n">
@@ -20136,7 +20136,7 @@
       </c>
       <c r="I379" t="inlineStr">
         <is>
-          <t>-0.21%</t>
+          <t>-0.22%</t>
         </is>
       </c>
       <c r="J379" t="n">
@@ -20188,7 +20188,7 @@
       </c>
       <c r="I380" t="inlineStr">
         <is>
-          <t>2.23%</t>
+          <t>2.39%</t>
         </is>
       </c>
       <c r="J380" t="n">
@@ -20240,7 +20240,7 @@
       </c>
       <c r="I381" t="inlineStr">
         <is>
-          <t>1.05%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J381" t="n">
@@ -20292,7 +20292,7 @@
       </c>
       <c r="I382" t="inlineStr">
         <is>
-          <t>0.31%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J382" t="n">
@@ -20344,7 +20344,7 @@
       </c>
       <c r="I383" t="inlineStr">
         <is>
-          <t>-0.84%</t>
+          <t>-1.36%</t>
         </is>
       </c>
       <c r="J383" t="n">
@@ -20396,7 +20396,7 @@
       </c>
       <c r="I384" t="inlineStr">
         <is>
-          <t>-0.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J384" t="n">
@@ -20448,7 +20448,7 @@
       </c>
       <c r="I385" t="inlineStr">
         <is>
-          <t>-0.35%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J385" t="n">
@@ -20500,7 +20500,7 @@
       </c>
       <c r="I386" t="inlineStr">
         <is>
-          <t>-0.6%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J386" t="n">
@@ -20552,7 +20552,7 @@
       </c>
       <c r="I387" t="inlineStr">
         <is>
-          <t>-0.41%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J387" t="n">
@@ -20604,7 +20604,7 @@
       </c>
       <c r="I388" t="inlineStr">
         <is>
-          <t>2.23%</t>
+          <t>2.48%</t>
         </is>
       </c>
       <c r="J388" t="n">
@@ -20656,7 +20656,7 @@
       </c>
       <c r="I389" t="inlineStr">
         <is>
-          <t>-3.07%</t>
+          <t>-2.99%</t>
         </is>
       </c>
       <c r="J389" t="n">
@@ -20708,7 +20708,7 @@
       </c>
       <c r="I390" t="inlineStr">
         <is>
-          <t>-0.23%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J390" t="n">
@@ -20760,7 +20760,7 @@
       </c>
       <c r="I391" t="inlineStr">
         <is>
-          <t>-0.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J391" t="n">
@@ -20812,7 +20812,7 @@
       </c>
       <c r="I392" t="inlineStr">
         <is>
-          <t>-1.72%</t>
+          <t>-1.96%</t>
         </is>
       </c>
       <c r="J392" t="n">
@@ -20864,7 +20864,7 @@
       </c>
       <c r="I393" t="inlineStr">
         <is>
-          <t>0.54%</t>
+          <t>0.82%</t>
         </is>
       </c>
       <c r="J393" t="n">
@@ -20916,7 +20916,7 @@
       </c>
       <c r="I394" t="inlineStr">
         <is>
-          <t>0.16%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J394" t="n">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="I395" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J395" t="n">
@@ -21020,7 +21020,7 @@
       </c>
       <c r="I396" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J396" t="n">
@@ -21072,7 +21072,7 @@
       </c>
       <c r="I397" t="inlineStr">
         <is>
-          <t>-0.16%</t>
+          <t>-0.5%</t>
         </is>
       </c>
       <c r="J397" t="n">
@@ -21124,7 +21124,7 @@
       </c>
       <c r="I398" t="inlineStr">
         <is>
-          <t>-0.82%</t>
+          <t>-2.56%</t>
         </is>
       </c>
       <c r="J398" t="n">
@@ -21176,7 +21176,7 @@
       </c>
       <c r="I399" t="inlineStr">
         <is>
-          <t>-0.27%</t>
+          <t>-0.98%</t>
         </is>
       </c>
       <c r="J399" t="n">
@@ -21228,7 +21228,7 @@
       </c>
       <c r="I400" t="inlineStr">
         <is>
-          <t>-1.07%</t>
+          <t>-0.79%</t>
         </is>
       </c>
       <c r="J400" t="n">
@@ -21280,7 +21280,7 @@
       </c>
       <c r="I401" t="inlineStr">
         <is>
-          <t>1.05%</t>
+          <t>0.83%</t>
         </is>
       </c>
       <c r="J401" t="n">
@@ -21332,7 +21332,7 @@
       </c>
       <c r="I402" t="inlineStr">
         <is>
-          <t>0.01%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J402" t="n">
@@ -21384,7 +21384,7 @@
       </c>
       <c r="I403" t="inlineStr">
         <is>
-          <t>2.66%</t>
+          <t>2.88%</t>
         </is>
       </c>
       <c r="J403" t="n">
@@ -21436,7 +21436,7 @@
       </c>
       <c r="I404" t="inlineStr">
         <is>
-          <t>-0.42%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J404" t="n">
@@ -21488,7 +21488,7 @@
       </c>
       <c r="I405" t="inlineStr">
         <is>
-          <t>-2.94%</t>
+          <t>-3.03%</t>
         </is>
       </c>
       <c r="J405" t="n">
@@ -21540,7 +21540,7 @@
       </c>
       <c r="I406" t="inlineStr">
         <is>
-          <t>0.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J406" t="n">
@@ -21592,7 +21592,7 @@
       </c>
       <c r="I407" t="inlineStr">
         <is>
-          <t>0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J407" t="n">
@@ -21644,7 +21644,7 @@
       </c>
       <c r="I408" t="inlineStr">
         <is>
-          <t>-1.58%</t>
+          <t>-2.9%</t>
         </is>
       </c>
       <c r="J408" t="n">
@@ -21696,7 +21696,7 @@
       </c>
       <c r="I409" t="inlineStr">
         <is>
-          <t>0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J409" t="n">
@@ -21748,7 +21748,7 @@
       </c>
       <c r="I410" t="inlineStr">
         <is>
-          <t>-0.73%</t>
+          <t>-0.77%</t>
         </is>
       </c>
       <c r="J410" t="n">
@@ -21800,7 +21800,7 @@
       </c>
       <c r="I411" t="inlineStr">
         <is>
-          <t>-1.33%</t>
+          <t>-1.9%</t>
         </is>
       </c>
       <c r="J411" t="n">
@@ -21852,7 +21852,7 @@
       </c>
       <c r="I412" t="inlineStr">
         <is>
-          <t>-1.18%</t>
+          <t>-1.02%</t>
         </is>
       </c>
       <c r="J412" t="n">
@@ -21904,7 +21904,7 @@
       </c>
       <c r="I413" t="inlineStr">
         <is>
-          <t>0.83%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J413" t="n">
@@ -21956,7 +21956,7 @@
       </c>
       <c r="I414" t="inlineStr">
         <is>
-          <t>0.13%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J414" t="n">
@@ -22008,7 +22008,7 @@
       </c>
       <c r="I415" t="inlineStr">
         <is>
-          <t>-0.29%</t>
+          <t>-0.93%</t>
         </is>
       </c>
       <c r="J415" t="n">
@@ -22060,7 +22060,7 @@
       </c>
       <c r="I416" t="inlineStr">
         <is>
-          <t>-1.51%</t>
+          <t>-1.28%</t>
         </is>
       </c>
       <c r="J416" t="n">
@@ -22112,7 +22112,7 @@
       </c>
       <c r="I417" t="inlineStr">
         <is>
-          <t>-0.78%</t>
+          <t>-0.61%</t>
         </is>
       </c>
       <c r="J417" t="n">
@@ -22164,7 +22164,7 @@
       </c>
       <c r="I418" t="inlineStr">
         <is>
-          <t>1.81%</t>
+          <t>1.95%</t>
         </is>
       </c>
       <c r="J418" t="n">
@@ -22216,7 +22216,7 @@
       </c>
       <c r="I419" t="inlineStr">
         <is>
-          <t>1.35%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="J419" t="n">
@@ -22268,7 +22268,7 @@
       </c>
       <c r="I420" t="inlineStr">
         <is>
-          <t>-0.68%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J420" t="n">
@@ -22320,7 +22320,7 @@
       </c>
       <c r="I421" t="inlineStr">
         <is>
-          <t>-1.72%</t>
+          <t>-4.0%</t>
         </is>
       </c>
       <c r="J421" t="n">
@@ -22372,7 +22372,7 @@
       </c>
       <c r="I422" t="inlineStr">
         <is>
-          <t>0.17%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J422" t="n">
@@ -22424,7 +22424,7 @@
       </c>
       <c r="I423" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>0.25%</t>
         </is>
       </c>
       <c r="J423" t="n">
@@ -22476,7 +22476,7 @@
       </c>
       <c r="I424" t="inlineStr">
         <is>
-          <t>0.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J424" t="n">
@@ -22528,7 +22528,7 @@
       </c>
       <c r="I425" t="inlineStr">
         <is>
-          <t>-1.99%</t>
+          <t>-2.33%</t>
         </is>
       </c>
       <c r="J425" t="n">
@@ -22580,7 +22580,7 @@
       </c>
       <c r="I426" t="inlineStr">
         <is>
-          <t>-0.58%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J426" t="n">
@@ -22632,7 +22632,7 @@
       </c>
       <c r="I427" t="inlineStr">
         <is>
-          <t>-1.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J427" t="n">
@@ -22684,7 +22684,7 @@
       </c>
       <c r="I428" t="inlineStr">
         <is>
-          <t>-0.05%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J428" t="n">
@@ -22736,7 +22736,7 @@
       </c>
       <c r="I429" t="inlineStr">
         <is>
-          <t>-1.61%</t>
+          <t>-1.85%</t>
         </is>
       </c>
       <c r="J429" t="n">
@@ -22788,7 +22788,7 @@
       </c>
       <c r="I430" t="inlineStr">
         <is>
-          <t>-2.67%</t>
+          <t>-3.23%</t>
         </is>
       </c>
       <c r="J430" t="n">
@@ -22840,7 +22840,7 @@
       </c>
       <c r="I431" t="inlineStr">
         <is>
-          <t>-2.36%</t>
+          <t>-4.55%</t>
         </is>
       </c>
       <c r="J431" t="n">
@@ -22892,7 +22892,7 @@
       </c>
       <c r="I432" t="inlineStr">
         <is>
-          <t>-0.21%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J432" t="n">
@@ -22944,7 +22944,7 @@
       </c>
       <c r="I433" t="inlineStr">
         <is>
-          <t>-0.49%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J433" t="n">
@@ -22996,7 +22996,7 @@
       </c>
       <c r="I434" t="inlineStr">
         <is>
-          <t>-0.05%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J434" t="n">
@@ -23048,7 +23048,7 @@
       </c>
       <c r="I435" t="inlineStr">
         <is>
-          <t>-0.32%</t>
+          <t>-1.61%</t>
         </is>
       </c>
       <c r="J435" t="n">
@@ -23100,7 +23100,7 @@
       </c>
       <c r="I436" t="inlineStr">
         <is>
-          <t>-2.29%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J436" t="n">
@@ -23152,7 +23152,7 @@
       </c>
       <c r="I437" t="inlineStr">
         <is>
-          <t>0.25%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J437" t="n">
@@ -23204,7 +23204,7 @@
       </c>
       <c r="I438" t="inlineStr">
         <is>
-          <t>-0.45%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J438" t="n">
@@ -23256,7 +23256,7 @@
       </c>
       <c r="I439" t="inlineStr">
         <is>
-          <t>-0.18%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J439" t="n">
@@ -23308,7 +23308,7 @@
       </c>
       <c r="I440" t="inlineStr">
         <is>
-          <t>-0.39%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J440" t="n">
@@ -23360,7 +23360,7 @@
       </c>
       <c r="I441" t="inlineStr">
         <is>
-          <t>-2.23%</t>
+          <t>-2.7%</t>
         </is>
       </c>
       <c r="J441" t="n">
@@ -23412,7 +23412,7 @@
       </c>
       <c r="I442" t="inlineStr">
         <is>
-          <t>-2.11%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J442" t="n">
@@ -23464,7 +23464,7 @@
       </c>
       <c r="I443" t="inlineStr">
         <is>
-          <t>1.03%</t>
+          <t>2.17%</t>
         </is>
       </c>
       <c r="J443" t="n">
@@ -23516,7 +23516,7 @@
       </c>
       <c r="I444" t="inlineStr">
         <is>
-          <t>-0.12%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J444" t="n">
@@ -23568,7 +23568,7 @@
       </c>
       <c r="I445" t="inlineStr">
         <is>
-          <t>-0.72%</t>
+          <t>-0.98%</t>
         </is>
       </c>
       <c r="J445" t="n">
@@ -23620,7 +23620,7 @@
       </c>
       <c r="I446" t="inlineStr">
         <is>
-          <t>-0.85%</t>
+          <t>-1.49%</t>
         </is>
       </c>
       <c r="J446" t="n">
@@ -23672,7 +23672,7 @@
       </c>
       <c r="I447" t="inlineStr">
         <is>
-          <t>-1.94%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J447" t="n">
@@ -23724,7 +23724,7 @@
       </c>
       <c r="I448" t="inlineStr">
         <is>
-          <t>0.52%</t>
+          <t>0.61%</t>
         </is>
       </c>
       <c r="J448" t="n">
@@ -23776,7 +23776,7 @@
       </c>
       <c r="I449" t="inlineStr">
         <is>
-          <t>-1.28%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J449" t="n">
@@ -23828,7 +23828,7 @@
       </c>
       <c r="I450" t="inlineStr">
         <is>
-          <t>-0.6%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J450" t="n">
@@ -23880,7 +23880,7 @@
       </c>
       <c r="I451" t="inlineStr">
         <is>
-          <t>0.57%</t>
+          <t>1.35%</t>
         </is>
       </c>
       <c r="J451" t="n">
@@ -23932,7 +23932,7 @@
       </c>
       <c r="I452" t="inlineStr">
         <is>
-          <t>-1.79%</t>
+          <t>-1.56%</t>
         </is>
       </c>
       <c r="J452" t="n">
@@ -23984,7 +23984,7 @@
       </c>
       <c r="I453" t="inlineStr">
         <is>
-          <t>-1.11%</t>
+          <t>-1.92%</t>
         </is>
       </c>
       <c r="J453" t="n">
@@ -24036,7 +24036,7 @@
       </c>
       <c r="I454" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J454" t="n">
@@ -24088,7 +24088,7 @@
       </c>
       <c r="I455" t="inlineStr">
         <is>
-          <t>0.01%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J455" t="n">
@@ -24140,7 +24140,7 @@
       </c>
       <c r="I456" t="inlineStr">
         <is>
-          <t>-2.0%</t>
+          <t>-1.72%</t>
         </is>
       </c>
       <c r="J456" t="n">
@@ -24192,7 +24192,7 @@
       </c>
       <c r="I457" t="inlineStr">
         <is>
-          <t>-0.88%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J457" t="n">
@@ -24244,7 +24244,7 @@
       </c>
       <c r="I458" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>0.82%</t>
         </is>
       </c>
       <c r="J458" t="n">
@@ -24296,7 +24296,7 @@
       </c>
       <c r="I459" t="inlineStr">
         <is>
-          <t>1.34%</t>
+          <t>2.08%</t>
         </is>
       </c>
       <c r="J459" t="n">
@@ -24348,7 +24348,7 @@
       </c>
       <c r="I460" t="inlineStr">
         <is>
-          <t>-2.31%</t>
+          <t>-1.41%</t>
         </is>
       </c>
       <c r="J460" t="n">
@@ -24400,7 +24400,7 @@
       </c>
       <c r="I461" t="inlineStr">
         <is>
-          <t>-0.7%</t>
+          <t>-2.33%</t>
         </is>
       </c>
       <c r="J461" t="n">
@@ -24452,7 +24452,7 @@
       </c>
       <c r="I462" t="inlineStr">
         <is>
-          <t>-1.41%</t>
+          <t>-2.78%</t>
         </is>
       </c>
       <c r="J462" t="n">
@@ -24504,7 +24504,7 @@
       </c>
       <c r="I463" t="inlineStr">
         <is>
-          <t>-0.34%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J463" t="n">
@@ -24556,7 +24556,7 @@
       </c>
       <c r="I464" t="inlineStr">
         <is>
-          <t>-0.08%</t>
+          <t>-0.89%</t>
         </is>
       </c>
       <c r="J464" t="n">
@@ -24608,7 +24608,7 @@
       </c>
       <c r="I465" t="inlineStr">
         <is>
-          <t>0.93%</t>
+          <t>0.56%</t>
         </is>
       </c>
       <c r="J465" t="n">
@@ -24660,7 +24660,7 @@
       </c>
       <c r="I466" t="inlineStr">
         <is>
-          <t>0.18%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J466" t="n">
@@ -24712,7 +24712,7 @@
       </c>
       <c r="I467" t="inlineStr">
         <is>
-          <t>-0.91%</t>
+          <t>-1.06%</t>
         </is>
       </c>
       <c r="J467" t="n">
@@ -24764,7 +24764,7 @@
       </c>
       <c r="I468" t="inlineStr">
         <is>
-          <t>-0.86%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J468" t="n">
@@ -24816,7 +24816,7 @@
       </c>
       <c r="I469" t="inlineStr">
         <is>
-          <t>-0.03%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J469" t="n">
@@ -24868,7 +24868,7 @@
       </c>
       <c r="I470" t="inlineStr">
         <is>
-          <t>-1.34%</t>
+          <t>-2.25%</t>
         </is>
       </c>
       <c r="J470" t="n">
@@ -24920,7 +24920,7 @@
       </c>
       <c r="I471" t="inlineStr">
         <is>
-          <t>-0.3%</t>
+          <t>-0.85%</t>
         </is>
       </c>
       <c r="J471" t="n">
@@ -24972,7 +24972,7 @@
       </c>
       <c r="I472" t="inlineStr">
         <is>
-          <t>-3.48%</t>
+          <t>-6.25%</t>
         </is>
       </c>
       <c r="J472" t="n">
@@ -25024,7 +25024,7 @@
       </c>
       <c r="I473" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J473" t="n">
@@ -25076,7 +25076,7 @@
       </c>
       <c r="I474" t="inlineStr">
         <is>
-          <t>-1.62%</t>
+          <t>-2.08%</t>
         </is>
       </c>
       <c r="J474" t="n">
@@ -25128,7 +25128,7 @@
       </c>
       <c r="I475" t="inlineStr">
         <is>
-          <t>0.53%</t>
+          <t>0.79%</t>
         </is>
       </c>
       <c r="J475" t="n">
@@ -25180,7 +25180,7 @@
       </c>
       <c r="I476" t="inlineStr">
         <is>
-          <t>4.48%</t>
+          <t>5.0%</t>
         </is>
       </c>
       <c r="J476" t="n">
@@ -25232,7 +25232,7 @@
       </c>
       <c r="I477" t="inlineStr">
         <is>
-          <t>0.12%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J477" t="n">
@@ -25284,7 +25284,7 @@
       </c>
       <c r="I478" t="inlineStr">
         <is>
-          <t>-1.3%</t>
+          <t>-1.18%</t>
         </is>
       </c>
       <c r="J478" t="n">
@@ -25336,7 +25336,7 @@
       </c>
       <c r="I479" t="inlineStr">
         <is>
-          <t>0.42%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J479" t="n">
@@ -25388,7 +25388,7 @@
       </c>
       <c r="I480" t="inlineStr">
         <is>
-          <t>-1.38%</t>
+          <t>-1.35%</t>
         </is>
       </c>
       <c r="J480" t="n">
@@ -25440,7 +25440,7 @@
       </c>
       <c r="I481" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J481" t="n">
@@ -25492,7 +25492,7 @@
       </c>
       <c r="I482" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J482" t="n">
@@ -25544,7 +25544,7 @@
       </c>
       <c r="I483" t="inlineStr">
         <is>
-          <t>-1.32%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J483" t="n">
@@ -25596,7 +25596,7 @@
       </c>
       <c r="I484" t="inlineStr">
         <is>
-          <t>1.94%</t>
+          <t>2.14%</t>
         </is>
       </c>
       <c r="J484" t="n">
@@ -25648,7 +25648,7 @@
       </c>
       <c r="I485" t="inlineStr">
         <is>
-          <t>0.21%</t>
+          <t>3.03%</t>
         </is>
       </c>
       <c r="J485" t="n">
@@ -25700,7 +25700,7 @@
       </c>
       <c r="I486" t="inlineStr">
         <is>
-          <t>-0.13%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J486" t="n">
@@ -25752,7 +25752,7 @@
       </c>
       <c r="I487" t="inlineStr">
         <is>
-          <t>-0.5%</t>
+          <t>-0.65%</t>
         </is>
       </c>
       <c r="J487" t="n">
@@ -25804,7 +25804,7 @@
       </c>
       <c r="I488" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>0.61%</t>
         </is>
       </c>
       <c r="J488" t="n">
@@ -25856,7 +25856,7 @@
       </c>
       <c r="I489" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J489" t="n">
@@ -25908,7 +25908,7 @@
       </c>
       <c r="I490" t="inlineStr">
         <is>
-          <t>-1.15%</t>
+          <t>-0.95%</t>
         </is>
       </c>
       <c r="J490" t="n">
@@ -25960,7 +25960,7 @@
       </c>
       <c r="I491" t="inlineStr">
         <is>
-          <t>-1.57%</t>
+          <t>-1.37%</t>
         </is>
       </c>
       <c r="J491" t="n">
@@ -26012,7 +26012,7 @@
       </c>
       <c r="I492" t="inlineStr">
         <is>
-          <t>-0.69%</t>
+          <t>-2.78%</t>
         </is>
       </c>
       <c r="J492" t="n">
@@ -26064,7 +26064,7 @@
       </c>
       <c r="I493" t="inlineStr">
         <is>
-          <t>-1.19%</t>
+          <t>-2.86%</t>
         </is>
       </c>
       <c r="J493" t="n">
@@ -26116,7 +26116,7 @@
       </c>
       <c r="I494" t="inlineStr">
         <is>
-          <t>0.46%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J494" t="n">
@@ -26168,7 +26168,7 @@
       </c>
       <c r="I495" t="inlineStr">
         <is>
-          <t>-1.48%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J495" t="n">
@@ -26220,7 +26220,7 @@
       </c>
       <c r="I496" t="inlineStr">
         <is>
-          <t>0.67%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J496" t="n">
@@ -26272,7 +26272,7 @@
       </c>
       <c r="I497" t="inlineStr">
         <is>
-          <t>-1.49%</t>
+          <t>-1.69%</t>
         </is>
       </c>
       <c r="J497" t="n">
@@ -26324,7 +26324,7 @@
       </c>
       <c r="I498" t="inlineStr">
         <is>
-          <t>-0.93%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J498" t="n">
@@ -26376,7 +26376,7 @@
       </c>
       <c r="I499" t="inlineStr">
         <is>
-          <t>3.42%</t>
+          <t>2.0%</t>
         </is>
       </c>
       <c r="J499" t="n">
@@ -26428,7 +26428,7 @@
       </c>
       <c r="I500" t="inlineStr">
         <is>
-          <t>-2.06%</t>
+          <t>-1.82%</t>
         </is>
       </c>
       <c r="J500" t="n">
@@ -26480,7 +26480,7 @@
       </c>
       <c r="I501" t="inlineStr">
         <is>
-          <t>-2.86%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J501" t="n">
@@ -26532,7 +26532,7 @@
       </c>
       <c r="I502" t="inlineStr">
         <is>
-          <t>-2.32%</t>
+          <t>-1.9%</t>
         </is>
       </c>
       <c r="J502" t="n">
@@ -26584,7 +26584,7 @@
       </c>
       <c r="I503" t="inlineStr">
         <is>
-          <t>-0.99%</t>
+          <t>-1.68%</t>
         </is>
       </c>
       <c r="J503" t="n">
@@ -26636,7 +26636,7 @@
       </c>
       <c r="I504" t="inlineStr">
         <is>
-          <t>-3.13%</t>
+          <t>-2.27%</t>
         </is>
       </c>
       <c r="J504" t="n">

</xml_diff>